<commit_message>
Update time management sheets
</commit_message>
<xml_diff>
--- a/man/group time management.xlsx
+++ b/man/group time management.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\Github\CS221\man\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="0" windowWidth="25080" windowHeight="1980"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -193,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -203,8 +198,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -225,7 +221,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -303,22 +299,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54166666666666674</c:v>
+                  <c:v>2.1736111111111107</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.2083333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>2.2291666666666665</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.58333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2.583333333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.27083333333333337</c:v>
+                  <c:v>1.8333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -336,11 +332,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="131436944"/>
-        <c:axId val="131434984"/>
+        <c:axId val="190496768"/>
+        <c:axId val="190498304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="131436944"/>
+        <c:axId val="190496768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -350,7 +346,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131434984"/>
+        <c:crossAx val="190498304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -358,7 +354,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131434984"/>
+        <c:axId val="190498304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -369,7 +365,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131436944"/>
+        <c:crossAx val="190496768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -389,7 +385,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -460,22 +456,22 @@
                   <c:v>3.3333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.791666666666667</c:v>
+                  <c:v>1.1597222222222228</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.3333333333333335</c:v>
+                  <c:v>2.125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.166666666666667</c:v>
+                  <c:v>1.104166666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3333333333333335</c:v>
+                  <c:v>2.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.3333333333333335</c:v>
+                  <c:v>0.75000000000000044</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0625</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.3333333333333335</c:v>
@@ -493,11 +489,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="292320256"/>
-        <c:axId val="292324176"/>
+        <c:axId val="190534784"/>
+        <c:axId val="190536320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292320256"/>
+        <c:axId val="190534784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -507,7 +503,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="292324176"/>
+        <c:crossAx val="190536320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -515,7 +511,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292324176"/>
+        <c:axId val="190536320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +522,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="292320256"/>
+        <c:crossAx val="190534784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -546,7 +542,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -614,22 +610,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54166666666666674</c:v>
+                  <c:v>2.1736111111111107</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.2083333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>2.2291666666666665</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.58333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2.583333333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.27083333333333337</c:v>
+                  <c:v>1.8333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -683,13 +679,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>404812</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>76205</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>156242</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -713,13 +709,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>66681</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>338137</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>142881</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -743,13 +739,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>47630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1323974</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -815,7 +811,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -850,7 +846,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1059,24 +1055,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CZ10"/>
+  <dimension ref="A1:CZ11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="10" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="11" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="14" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="22" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="22" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:104" ht="18" x14ac:dyDescent="0.35">
@@ -1155,32 +1153,35 @@
         <v>1</v>
       </c>
       <c r="C2" s="7">
-        <f>(B10-D2)</f>
+        <f>(B11-D2)</f>
         <v>3.3333333333333335</v>
       </c>
       <c r="D2" s="7">
-        <f>SUM(G2:CZ2)</f>
+        <f t="shared" ref="D2:D9" si="0">SUM(F2:CZ2)</f>
         <v>0</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="G2" s="8">
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10">
         <v>0</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
+      <c r="P2" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
       <c r="W2" s="8"/>
       <c r="X2" s="8"/>
       <c r="Y2" s="8"/>
@@ -1272,34 +1273,55 @@
         <v>3</v>
       </c>
       <c r="C3" s="7">
-        <f>(B10-D3)</f>
-        <v>2.791666666666667</v>
+        <f>(B11-D3)</f>
+        <v>1.1597222222222228</v>
       </c>
       <c r="D3" s="7">
-        <f>SUM(G3:CZ3)</f>
-        <v>0.54166666666666674</v>
+        <f t="shared" si="0"/>
+        <v>2.1736111111111107</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="G3" s="8">
+      <c r="F3" s="10">
         <v>0.41666666666666669</v>
       </c>
-      <c r="H3" s="8">
+      <c r="G3" s="10">
         <v>0.125</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
+      <c r="H3" s="10">
+        <v>0.125</v>
+      </c>
+      <c r="I3" s="10">
+        <v>9.375E-2</v>
+      </c>
+      <c r="J3" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="K3" s="10">
+        <v>0.15625</v>
+      </c>
+      <c r="L3" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="M3" s="10">
+        <v>0.15277777777777776</v>
+      </c>
+      <c r="N3" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="O3" s="10">
+        <v>0</v>
+      </c>
+      <c r="P3" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>1</v>
+      </c>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
       <c r="W3" s="8"/>
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
@@ -1391,32 +1413,46 @@
         <v>5</v>
       </c>
       <c r="C4" s="7">
-        <f>(B10-D4)</f>
-        <v>3.3333333333333335</v>
+        <f>(B11-D4)</f>
+        <v>2.125</v>
       </c>
       <c r="D4" s="7">
-        <f>SUM(G4:CZ4)</f>
+        <f t="shared" si="0"/>
+        <v>1.2083333333333333</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="10">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="G4" s="10">
+        <v>6.25E-2</v>
+      </c>
+      <c r="H4" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="I4" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K4" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="L4" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="O4" s="10">
         <v>0</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="G4" s="8">
+      <c r="P4" s="10">
         <v>0</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
+      <c r="Q4" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
@@ -1508,32 +1544,55 @@
         <v>7</v>
       </c>
       <c r="C5" s="7">
-        <f>(B10-D5)</f>
-        <v>3.166666666666667</v>
+        <f>(B11-D5)</f>
+        <v>1.104166666666667</v>
       </c>
       <c r="D5" s="7">
-        <f>SUM(G5:CZ5)</f>
+        <f t="shared" si="0"/>
+        <v>2.2291666666666665</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="10">
         <v>0.16666666666666666</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="G5" s="8">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
+      <c r="G5" s="10">
+        <v>0.125</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="I5" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="K5" s="10">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="L5" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="M5" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="N5" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="O5" s="10">
+        <v>0</v>
+      </c>
+      <c r="P5" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
       <c r="W5" s="8"/>
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
@@ -1625,32 +1684,41 @@
         <v>9</v>
       </c>
       <c r="C6" s="7">
-        <f>(B10-D6)</f>
-        <v>3.3333333333333335</v>
+        <f>(B11-D6)</f>
+        <v>2.75</v>
       </c>
       <c r="D6" s="7">
-        <f>SUM(G6:CZ6)</f>
+        <f t="shared" si="0"/>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="I6" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10">
         <v>0</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="G6" s="8">
+      <c r="P6" s="10">
         <v>0</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
@@ -1742,32 +1810,51 @@
         <v>11</v>
       </c>
       <c r="C7" s="7">
-        <f>(B10-D7)</f>
-        <v>3.3333333333333335</v>
+        <f>(B11-D7)</f>
+        <v>0.75000000000000044</v>
       </c>
       <c r="D7" s="7">
-        <f>SUM(G7:CZ7)</f>
+        <f t="shared" si="0"/>
+        <v>2.583333333333333</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I7" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J7" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K7" s="10">
         <v>0</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="G7" s="8">
+      <c r="L7" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="M7" s="10">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10">
         <v>0</v>
       </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
+      <c r="P7" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="10">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8"/>
       <c r="Y7" s="8"/>
@@ -1859,34 +1946,55 @@
         <v>13</v>
       </c>
       <c r="C8" s="7">
-        <f>(B10-D8)</f>
-        <v>3.0625</v>
+        <f>(B11-D8)</f>
+        <v>1.5</v>
       </c>
       <c r="D8" s="7">
-        <f>SUM(G8:CZ8)</f>
-        <v>0.27083333333333337</v>
+        <f t="shared" si="0"/>
+        <v>1.8333333333333335</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="G8" s="8">
+      <c r="F8" s="10">
         <v>3.125E-2</v>
       </c>
-      <c r="H8" s="8">
+      <c r="G8" s="10">
         <v>0.23958333333333334</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
+      <c r="H8" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="I8" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0.125</v>
+      </c>
+      <c r="L8" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="M8" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="N8" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="O8" s="10">
+        <v>0</v>
+      </c>
+      <c r="P8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
       <c r="W8" s="8"/>
       <c r="X8" s="8"/>
       <c r="Y8" s="8"/>
@@ -1978,32 +2086,35 @@
         <v>15</v>
       </c>
       <c r="C9" s="7">
-        <f>(B10-D9)</f>
+        <f>(B11-D9)</f>
         <v>3.3333333333333335</v>
       </c>
       <c r="D9" s="7">
-        <f>SUM(G9:CZ9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="G9" s="8">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10">
         <v>0</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
+      <c r="P9" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
       <c r="W9" s="8"/>
       <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
@@ -2087,123 +2198,229 @@
       <c r="CY9" s="8"/>
       <c r="CZ9" s="8"/>
     </row>
-    <row r="10" spans="1:104" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:104" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8"/>
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="8"/>
+      <c r="AG10" s="8"/>
+      <c r="AH10" s="8"/>
+      <c r="AI10" s="8"/>
+      <c r="AJ10" s="8"/>
+      <c r="AK10" s="8"/>
+      <c r="AL10" s="8"/>
+      <c r="AM10" s="8"/>
+      <c r="AN10" s="8"/>
+      <c r="AO10" s="8"/>
+      <c r="AP10" s="8"/>
+      <c r="AQ10" s="8"/>
+      <c r="AR10" s="8"/>
+      <c r="AS10" s="8"/>
+      <c r="AT10" s="8"/>
+      <c r="AU10" s="8"/>
+      <c r="AV10" s="8"/>
+      <c r="AW10" s="8"/>
+      <c r="AX10" s="8"/>
+      <c r="AY10" s="8"/>
+      <c r="AZ10" s="8"/>
+      <c r="BA10" s="8"/>
+      <c r="BB10" s="8"/>
+      <c r="BC10" s="8"/>
+      <c r="BD10" s="8"/>
+      <c r="BE10" s="8"/>
+      <c r="BF10" s="8"/>
+      <c r="BG10" s="8"/>
+      <c r="BH10" s="8"/>
+      <c r="BI10" s="8"/>
+      <c r="BJ10" s="8"/>
+      <c r="BK10" s="8"/>
+      <c r="BL10" s="8"/>
+      <c r="BM10" s="8"/>
+      <c r="BN10" s="8"/>
+      <c r="BO10" s="8"/>
+      <c r="BP10" s="8"/>
+      <c r="BQ10" s="8"/>
+      <c r="BR10" s="8"/>
+      <c r="BS10" s="8"/>
+      <c r="BT10" s="8"/>
+      <c r="BU10" s="8"/>
+      <c r="BV10" s="8"/>
+      <c r="BW10" s="8"/>
+      <c r="BX10" s="8"/>
+      <c r="BY10" s="8"/>
+      <c r="BZ10" s="8"/>
+      <c r="CA10" s="8"/>
+      <c r="CB10" s="8"/>
+      <c r="CC10" s="8"/>
+      <c r="CD10" s="8"/>
+      <c r="CE10" s="8"/>
+      <c r="CF10" s="8"/>
+      <c r="CG10" s="8"/>
+      <c r="CH10" s="8"/>
+      <c r="CI10" s="8"/>
+      <c r="CJ10" s="8"/>
+      <c r="CK10" s="8"/>
+      <c r="CL10" s="8"/>
+      <c r="CM10" s="8"/>
+      <c r="CN10" s="8"/>
+      <c r="CO10" s="8"/>
+      <c r="CP10" s="8"/>
+      <c r="CQ10" s="8"/>
+      <c r="CR10" s="8"/>
+      <c r="CS10" s="8"/>
+      <c r="CT10" s="8"/>
+      <c r="CU10" s="8"/>
+      <c r="CV10" s="8"/>
+      <c r="CW10" s="8"/>
+      <c r="CX10" s="8"/>
+      <c r="CY10" s="8"/>
+      <c r="CZ10" s="8"/>
+    </row>
+    <row r="11" spans="1:104" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B11" s="6">
         <v>3.3333333333333335</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D11" s="9">
         <f>SUM(D2:D9)</f>
-        <v>0.97916666666666674</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
-      <c r="AA10" s="9"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="9"/>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="9"/>
-      <c r="AF10" s="9"/>
-      <c r="AG10" s="9"/>
-      <c r="AH10" s="9"/>
-      <c r="AI10" s="9"/>
-      <c r="AJ10" s="9"/>
-      <c r="AK10" s="9"/>
-      <c r="AL10" s="9"/>
-      <c r="AM10" s="9"/>
-      <c r="AN10" s="9"/>
-      <c r="AO10" s="9"/>
-      <c r="AP10" s="9"/>
-      <c r="AQ10" s="9"/>
-      <c r="AR10" s="9"/>
-      <c r="AS10" s="9"/>
-      <c r="AT10" s="9"/>
-      <c r="AU10" s="9"/>
-      <c r="AV10" s="9"/>
-      <c r="AW10" s="9"/>
-      <c r="AX10" s="9"/>
-      <c r="AY10" s="9"/>
-      <c r="AZ10" s="9"/>
-      <c r="BA10" s="9"/>
-      <c r="BB10" s="9"/>
-      <c r="BC10" s="9"/>
-      <c r="BD10" s="9"/>
-      <c r="BE10" s="9"/>
-      <c r="BF10" s="9"/>
-      <c r="BG10" s="9"/>
-      <c r="BH10" s="9"/>
-      <c r="BI10" s="9"/>
-      <c r="BJ10" s="9"/>
-      <c r="BK10" s="9"/>
-      <c r="BL10" s="9"/>
-      <c r="BM10" s="9"/>
-      <c r="BN10" s="9"/>
-      <c r="BO10" s="9"/>
-      <c r="BP10" s="9"/>
-      <c r="BQ10" s="9"/>
-      <c r="BR10" s="9"/>
-      <c r="BS10" s="9"/>
-      <c r="BT10" s="9"/>
-      <c r="BU10" s="9"/>
-      <c r="BV10" s="9"/>
-      <c r="BW10" s="9"/>
-      <c r="BX10" s="9"/>
-      <c r="BY10" s="9"/>
-      <c r="BZ10" s="9"/>
-      <c r="CA10" s="9"/>
-      <c r="CB10" s="9"/>
-      <c r="CC10" s="9"/>
-      <c r="CD10" s="9"/>
-      <c r="CE10" s="9"/>
-      <c r="CF10" s="9"/>
-      <c r="CG10" s="9"/>
-      <c r="CH10" s="9"/>
-      <c r="CI10" s="9"/>
-      <c r="CJ10" s="9"/>
-      <c r="CK10" s="9"/>
-      <c r="CL10" s="9"/>
-      <c r="CM10" s="9"/>
-      <c r="CN10" s="9"/>
-      <c r="CO10" s="9"/>
-      <c r="CP10" s="9"/>
-      <c r="CQ10" s="9"/>
-      <c r="CR10" s="9"/>
-      <c r="CS10" s="9"/>
-      <c r="CT10" s="9"/>
-      <c r="CU10" s="9"/>
-      <c r="CV10" s="9"/>
-      <c r="CW10" s="9"/>
-      <c r="CX10" s="9"/>
-      <c r="CY10" s="9"/>
+        <v>10.611111111111111</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="11"/>
+      <c r="AG11" s="11"/>
+      <c r="AH11" s="11"/>
+      <c r="AI11" s="11"/>
+      <c r="AJ11" s="11"/>
+      <c r="AK11" s="11"/>
+      <c r="AL11" s="11"/>
+      <c r="AM11" s="11"/>
+      <c r="AN11" s="11"/>
+      <c r="AO11" s="11"/>
+      <c r="AP11" s="11"/>
+      <c r="AQ11" s="11"/>
+      <c r="AR11" s="11"/>
+      <c r="AS11" s="11"/>
+      <c r="AT11" s="11"/>
+      <c r="AU11" s="11"/>
+      <c r="AV11" s="11"/>
+      <c r="AW11" s="11"/>
+      <c r="AX11" s="11"/>
+      <c r="AY11" s="11"/>
+      <c r="AZ11" s="11"/>
+      <c r="BA11" s="11"/>
+      <c r="BB11" s="11"/>
+      <c r="BC11" s="11"/>
+      <c r="BD11" s="11"/>
+      <c r="BE11" s="11"/>
+      <c r="BF11" s="11"/>
+      <c r="BG11" s="11"/>
+      <c r="BH11" s="11"/>
+      <c r="BI11" s="11"/>
+      <c r="BJ11" s="11"/>
+      <c r="BK11" s="11"/>
+      <c r="BL11" s="11"/>
+      <c r="BM11" s="11"/>
+      <c r="BN11" s="11"/>
+      <c r="BO11" s="11"/>
+      <c r="BP11" s="11"/>
+      <c r="BQ11" s="11"/>
+      <c r="BR11" s="11"/>
+      <c r="BS11" s="11"/>
+      <c r="BT11" s="11"/>
+      <c r="BU11" s="11"/>
+      <c r="BV11" s="11"/>
+      <c r="BW11" s="11"/>
+      <c r="BX11" s="11"/>
+      <c r="BY11" s="11"/>
+      <c r="BZ11" s="11"/>
+      <c r="CA11" s="11"/>
+      <c r="CB11" s="11"/>
+      <c r="CC11" s="11"/>
+      <c r="CD11" s="11"/>
+      <c r="CE11" s="11"/>
+      <c r="CF11" s="11"/>
+      <c r="CG11" s="11"/>
+      <c r="CH11" s="11"/>
+      <c r="CI11" s="11"/>
+      <c r="CJ11" s="11"/>
+      <c r="CK11" s="11"/>
+      <c r="CL11" s="11"/>
+      <c r="CM11" s="11"/>
+      <c r="CN11" s="11"/>
+      <c r="CO11" s="11"/>
+      <c r="CP11" s="11"/>
+      <c r="CQ11" s="11"/>
+      <c r="CR11" s="11"/>
+      <c r="CS11" s="11"/>
+      <c r="CT11" s="11"/>
+      <c r="CU11" s="11"/>
+      <c r="CV11" s="11"/>
+      <c r="CW11" s="11"/>
+      <c r="CX11" s="11"/>
+      <c r="CY11" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E10:CY10"/>
+    <mergeCell ref="E11:CY11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2217,7 +2434,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2229,7 +2446,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Ben's Time sheets
</commit_message>
<xml_diff>
--- a/man/group time management.xlsx
+++ b/man/group time management.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="0" windowWidth="25080" windowHeight="1980"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Ben Dudley</t>
   </si>
@@ -121,18 +121,6 @@
   </si>
   <si>
     <t>Wk 13</t>
-  </si>
-  <si>
-    <t>Wk 14</t>
-  </si>
-  <si>
-    <t>Wk 15</t>
-  </si>
-  <si>
-    <t>Wk 16</t>
-  </si>
-  <si>
-    <t>Wk 17</t>
   </si>
   <si>
     <t>Total Hours</t>
@@ -220,7 +208,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
+  <c:date1904 val="1"/>
   <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -296,7 +284,7 @@
                 <c:formatCode>[h]:mm</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2.2083333333333335</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.1736111111111107</c:v>
@@ -384,7 +372,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
+  <c:date1904 val="1"/>
   <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -453,28 +441,28 @@
                 <c:formatCode>[h]:mm</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3.3333333333333335</c:v>
+                  <c:v>-0.54166666666666674</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1597222222222228</c:v>
+                  <c:v>-0.50694444444444398</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.125</c:v>
+                  <c:v>0.45833333333333348</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.104166666666667</c:v>
+                  <c:v>-0.56249999999999978</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.75</c:v>
+                  <c:v>1.0833333333333335</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.75000000000000044</c:v>
+                  <c:v>-0.9166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5</c:v>
+                  <c:v>-0.16666666666666674</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.3333333333333335</c:v>
+                  <c:v>1.6666666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -541,7 +529,7 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
+  <c:date1904 val="1"/>
   <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -607,7 +595,7 @@
                 <c:formatCode>[h]:mm</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2.2083333333333335</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.1736111111111107</c:v>
@@ -1061,14 +1049,14 @@
       <pane xSplit="4" ySplit="11" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomRight" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
@@ -1132,18 +1120,10 @@
       <c r="R1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
     </row>
     <row r="2" spans="1:104" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -1154,29 +1134,49 @@
       </c>
       <c r="C2" s="7">
         <f>(B11-D2)</f>
-        <v>3.3333333333333335</v>
+        <v>-0.54166666666666674</v>
       </c>
       <c r="D2" s="7">
         <f t="shared" ref="D2:D9" si="0">SUM(F2:CZ2)</f>
-        <v>0</v>
+        <v>2.2083333333333335</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
+      <c r="F2" s="10">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H2" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="J2" s="10">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="K2" s="10">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="L2" s="10">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="M2" s="10">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="N2" s="10">
+        <v>6.25E-2</v>
+      </c>
       <c r="O2" s="10">
         <v>0</v>
       </c>
       <c r="P2" s="10">
         <v>0</v>
       </c>
-      <c r="Q2" s="10"/>
+      <c r="Q2" s="10">
+        <v>0.5625</v>
+      </c>
       <c r="R2" s="10"/>
       <c r="S2" s="10"/>
       <c r="T2" s="10"/>
@@ -1274,7 +1274,7 @@
       </c>
       <c r="C3" s="7">
         <f>(B11-D3)</f>
-        <v>1.1597222222222228</v>
+        <v>-0.50694444444444398</v>
       </c>
       <c r="D3" s="7">
         <f t="shared" si="0"/>
@@ -1414,7 +1414,7 @@
       </c>
       <c r="C4" s="7">
         <f>(B11-D4)</f>
-        <v>2.125</v>
+        <v>0.45833333333333348</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" si="0"/>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="C5" s="7">
         <f>(B11-D5)</f>
-        <v>1.104166666666667</v>
+        <v>-0.56249999999999978</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="C6" s="7">
         <f>(B11-D6)</f>
-        <v>2.75</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="D6" s="7">
         <f t="shared" si="0"/>
@@ -1811,14 +1811,16 @@
       </c>
       <c r="C7" s="7">
         <f>(B11-D7)</f>
-        <v>0.75000000000000044</v>
+        <v>-0.9166666666666663</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" si="0"/>
         <v>2.583333333333333</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="10"/>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
       <c r="G7" s="10">
         <v>0.70833333333333337</v>
       </c>
@@ -1840,7 +1842,9 @@
       <c r="M7" s="10">
         <v>0.20833333333333334</v>
       </c>
-      <c r="N7" s="10"/>
+      <c r="N7" s="10">
+        <v>0</v>
+      </c>
       <c r="O7" s="10">
         <v>0</v>
       </c>
@@ -1947,7 +1951,7 @@
       </c>
       <c r="C8" s="7">
         <f>(B11-D8)</f>
-        <v>1.5</v>
+        <v>-0.16666666666666674</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" si="0"/>
@@ -2087,7 +2091,7 @@
       </c>
       <c r="C9" s="7">
         <f>(B11-D9)</f>
-        <v>3.3333333333333335</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" si="0"/>
@@ -2309,14 +2313,14 @@
         <v>20</v>
       </c>
       <c r="B11" s="6">
-        <v>3.3333333333333335</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D11" s="9">
         <f>SUM(D2:D9)</f>
-        <v>10.611111111111111</v>
+        <v>12.819444444444445</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>

</xml_diff>

<commit_message>
Compiled final report, tided repo and copied libraries into lib
</commit_message>
<xml_diff>
--- a/man/group time management.xlsx
+++ b/man/group time management.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\Github\cs221\man\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="0" windowWidth="25080" windowHeight="1980"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -214,7 +209,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -295,7 +290,7 @@
                   <c:v>3.4861111111111107</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9583333333333333</c:v>
+                  <c:v>2.625</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3.4375</c:v>
@@ -325,11 +320,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="141090040"/>
-        <c:axId val="141090824"/>
+        <c:axId val="195284352"/>
+        <c:axId val="124236928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141090040"/>
+        <c:axId val="195284352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -339,7 +334,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141090824"/>
+        <c:crossAx val="124236928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -347,7 +342,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141090824"/>
+        <c:axId val="124236928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -358,7 +353,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141090040"/>
+        <c:crossAx val="195284352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -378,7 +373,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -452,7 +447,7 @@
                   <c:v>-0.15277777777777724</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3750000000000002</c:v>
+                  <c:v>0.70833333333333348</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>-0.10416666666666652</c:v>
@@ -482,11 +477,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="297716784"/>
-        <c:axId val="297719136"/>
+        <c:axId val="124596992"/>
+        <c:axId val="124598528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="297716784"/>
+        <c:axId val="124596992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,7 +491,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297719136"/>
+        <c:crossAx val="124598528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -504,7 +499,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297719136"/>
+        <c:axId val="124598528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,7 +510,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297716784"/>
+        <c:crossAx val="124596992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -535,7 +530,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -606,7 +601,7 @@
                   <c:v>3.4861111111111107</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9583333333333333</c:v>
+                  <c:v>2.625</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3.4375</c:v>
@@ -804,7 +799,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -839,7 +834,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1054,20 +1049,20 @@
       <pane xSplit="4" ySplit="11" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="14" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="22" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:104" ht="18" x14ac:dyDescent="0.35">
@@ -1421,11 +1416,11 @@
       </c>
       <c r="C4" s="7">
         <f>(B11-D4)</f>
-        <v>1.3750000000000002</v>
+        <v>0.70833333333333348</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" si="0"/>
-        <v>1.9583333333333333</v>
+        <v>2.625</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="10">
@@ -1455,7 +1450,9 @@
       <c r="Q4" s="8">
         <v>1.5</v>
       </c>
-      <c r="R4" s="10"/>
+      <c r="R4" s="10">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
@@ -2344,7 +2341,7 @@
       </c>
       <c r="D11" s="9">
         <f>SUM(D2:D9)</f>
-        <v>19.215277777777779</v>
+        <v>19.881944444444443</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -2462,7 +2459,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2474,7 +2471,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>